<commit_message>
Bump version to 2.4
</commit_message>
<xml_diff>
--- a/stat/downloads.xlsx
+++ b/stat/downloads.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="460" windowWidth="17820" windowHeight="26000"/>
+    <workbookView xWindow="-25880" yWindow="460" windowWidth="17820" windowHeight="26000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="117">
   <si>
     <t>ダウンロード数(累計)</t>
   </si>
@@ -356,6 +356,65 @@
   </si>
   <si>
     <t>2019/01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2019/02</t>
+  </si>
+  <si>
+    <t>2019/03</t>
+  </si>
+  <si>
+    <t>2019/04</t>
+  </si>
+  <si>
+    <t>2019/05</t>
+  </si>
+  <si>
+    <t>2019/06</t>
+  </si>
+  <si>
+    <t>2019/07</t>
+  </si>
+  <si>
+    <t>2019/08</t>
+  </si>
+  <si>
+    <t>2019/09</t>
+  </si>
+  <si>
+    <t>2019/10</t>
+  </si>
+  <si>
+    <t>2019/11</t>
+  </si>
+  <si>
+    <t>2019/12</t>
+  </si>
+  <si>
+    <t>DSQSS 講習会</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MateriApps LIVE!講習会</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バージョン2.4公開
+xTAPP, Dcore講習会</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バージョン2.3公開
+ALAMODE講習会</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バージョン2.2公開</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>講習会＠ブラジル</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1703,13 +1762,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C69" sqref="C69:C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="14.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2522,11 +2581,11 @@
         <v>54</v>
       </c>
       <c r="B35" s="1">
-        <f t="shared" ref="B35:B68" si="2">B34+D35</f>
+        <f t="shared" ref="B35:B79" si="2">B34+D35</f>
         <v>1660</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" ref="C35:C68" si="3">C34+E35</f>
+        <f t="shared" ref="C35:C79" si="3">C34+E35</f>
         <v>530</v>
       </c>
       <c r="D35" s="3">
@@ -3258,6 +3317,209 @@
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A69" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B69" s="9">
+        <f t="shared" si="2"/>
+        <v>4442</v>
+      </c>
+      <c r="C69" s="9">
+        <f t="shared" si="3"/>
+        <v>702</v>
+      </c>
+      <c r="D69" s="1">
+        <v>102</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A70" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B70" s="9">
+        <f t="shared" si="2"/>
+        <v>4546</v>
+      </c>
+      <c r="C70" s="9">
+        <f t="shared" si="3"/>
+        <v>702</v>
+      </c>
+      <c r="D70" s="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A71" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B71" s="9">
+        <f t="shared" si="2"/>
+        <v>4731</v>
+      </c>
+      <c r="C71" s="9">
+        <f t="shared" si="3"/>
+        <v>772</v>
+      </c>
+      <c r="D71" s="1">
+        <v>185</v>
+      </c>
+      <c r="E71" s="1">
+        <v>70</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="28" x14ac:dyDescent="0.15">
+      <c r="A72" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B72" s="9">
+        <f t="shared" si="2"/>
+        <v>4922</v>
+      </c>
+      <c r="C72" s="9">
+        <f t="shared" si="3"/>
+        <v>772</v>
+      </c>
+      <c r="D72" s="1">
+        <v>191</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A73" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B73" s="9">
+        <f t="shared" si="2"/>
+        <v>5005</v>
+      </c>
+      <c r="C73" s="9">
+        <f t="shared" si="3"/>
+        <v>772</v>
+      </c>
+      <c r="D73" s="1">
+        <v>83</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A74" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B74" s="9">
+        <f t="shared" si="2"/>
+        <v>5094</v>
+      </c>
+      <c r="C74" s="9">
+        <f t="shared" si="3"/>
+        <v>792</v>
+      </c>
+      <c r="D74" s="1">
+        <v>89</v>
+      </c>
+      <c r="E74" s="1">
+        <v>20</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A75" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B75" s="9">
+        <f t="shared" si="2"/>
+        <v>5195</v>
+      </c>
+      <c r="C75" s="9">
+        <f t="shared" si="3"/>
+        <v>792</v>
+      </c>
+      <c r="D75" s="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A76" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B76" s="9">
+        <f t="shared" si="2"/>
+        <v>5344</v>
+      </c>
+      <c r="C76" s="9">
+        <f t="shared" si="3"/>
+        <v>792</v>
+      </c>
+      <c r="D76" s="1">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A77" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B77" s="9">
+        <f t="shared" si="2"/>
+        <v>5531</v>
+      </c>
+      <c r="C77" s="9">
+        <f t="shared" si="3"/>
+        <v>792</v>
+      </c>
+      <c r="D77" s="1">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A78" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B78" s="9">
+        <f t="shared" si="2"/>
+        <v>5644</v>
+      </c>
+      <c r="C78" s="9">
+        <f t="shared" si="3"/>
+        <v>800</v>
+      </c>
+      <c r="D78" s="1">
+        <v>113</v>
+      </c>
+      <c r="E78" s="1">
+        <v>8</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="28" x14ac:dyDescent="0.15">
+      <c r="A79" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B79" s="9">
+        <f t="shared" si="2"/>
+        <v>5644</v>
+      </c>
+      <c r="C79" s="9">
+        <f t="shared" si="3"/>
+        <v>800</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
remove buster support, preparing for ma5
</commit_message>
<xml_diff>
--- a/stat/downloads.xlsx
+++ b/stat/downloads.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wistaria/Library/CloudStorage/Dropbox/development/ma/MateriAppsLive/stat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30BA553-13C5-B04E-938B-FC71D72D32B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE8C7ED-67F8-274A-A4EB-57C811D5BE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,7 +815,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
@@ -2008,10 +2008,10 @@
   <dimension ref="A1:M139"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B107" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B96" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G131" sqref="G131"/>
+      <selection pane="bottomRight" activeCell="B116" sqref="B116:B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3050,11 +3050,11 @@
         <v>2190</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" ref="C35:C115" si="3">C34+E35</f>
+        <f t="shared" ref="C35:C116" si="3">C34+E35</f>
         <v>1660</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" ref="D35:D115" si="4">D34+F35</f>
+        <f t="shared" ref="D35:D116" si="4">D34+F35</f>
         <v>530</v>
       </c>
       <c r="E35" s="3">
@@ -3104,7 +3104,7 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
         <v>57</v>
       </c>
@@ -4993,15 +4993,18 @@
       </c>
       <c r="B115" s="1">
         <f>C115+D115+G115</f>
-        <v>15145</v>
+        <v>15259</v>
       </c>
       <c r="C115" s="9">
         <f t="shared" si="3"/>
-        <v>13971</v>
+        <v>14085</v>
       </c>
       <c r="D115" s="9">
         <f t="shared" si="4"/>
         <v>959</v>
+      </c>
+      <c r="E115" s="1">
+        <v>114</v>
       </c>
       <c r="G115" s="1">
         <v>215</v>
@@ -5011,6 +5014,21 @@
       <c r="A116" s="8" t="s">
         <v>159</v>
       </c>
+      <c r="B116" s="1">
+        <f t="shared" ref="B116:B133" si="6">C116+D116+G116</f>
+        <v>15467</v>
+      </c>
+      <c r="C116" s="9">
+        <f t="shared" si="3"/>
+        <v>14273</v>
+      </c>
+      <c r="D116" s="9">
+        <f t="shared" si="4"/>
+        <v>959</v>
+      </c>
+      <c r="E116" s="1">
+        <v>188</v>
+      </c>
       <c r="G116" s="1">
         <v>235</v>
       </c>
@@ -5019,6 +5037,21 @@
       <c r="A117" s="8" t="s">
         <v>160</v>
       </c>
+      <c r="B117" s="1">
+        <f t="shared" si="6"/>
+        <v>15587</v>
+      </c>
+      <c r="C117" s="9">
+        <f t="shared" ref="C117:D133" si="7">C116+E117</f>
+        <v>14387</v>
+      </c>
+      <c r="D117" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E117" s="1">
+        <v>114</v>
+      </c>
       <c r="G117" s="1">
         <v>241</v>
       </c>
@@ -5027,6 +5060,21 @@
       <c r="A118" s="8" t="s">
         <v>161</v>
       </c>
+      <c r="B118" s="1">
+        <f t="shared" si="6"/>
+        <v>15978</v>
+      </c>
+      <c r="C118" s="9">
+        <f t="shared" si="7"/>
+        <v>14650</v>
+      </c>
+      <c r="D118" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E118" s="1">
+        <v>263</v>
+      </c>
       <c r="G118" s="1">
         <v>369</v>
       </c>
@@ -5035,6 +5083,21 @@
       <c r="A119" s="8" t="s">
         <v>162</v>
       </c>
+      <c r="B119" s="1">
+        <f t="shared" si="6"/>
+        <v>16236</v>
+      </c>
+      <c r="C119" s="9">
+        <f t="shared" si="7"/>
+        <v>14866</v>
+      </c>
+      <c r="D119" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E119" s="1">
+        <v>216</v>
+      </c>
       <c r="G119" s="1">
         <v>411</v>
       </c>
@@ -5043,6 +5106,21 @@
       <c r="A120" s="8" t="s">
         <v>163</v>
       </c>
+      <c r="B120" s="1">
+        <f t="shared" si="6"/>
+        <v>16519</v>
+      </c>
+      <c r="C120" s="9">
+        <f t="shared" si="7"/>
+        <v>15129</v>
+      </c>
+      <c r="D120" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E120" s="1">
+        <v>263</v>
+      </c>
       <c r="G120" s="1">
         <v>431</v>
       </c>
@@ -5051,6 +5129,21 @@
       <c r="A121" s="8" t="s">
         <v>164</v>
       </c>
+      <c r="B121" s="1">
+        <f t="shared" si="6"/>
+        <v>16792</v>
+      </c>
+      <c r="C121" s="9">
+        <f t="shared" si="7"/>
+        <v>15396</v>
+      </c>
+      <c r="D121" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E121" s="1">
+        <v>267</v>
+      </c>
       <c r="G121" s="1">
         <v>437</v>
       </c>
@@ -5059,6 +5152,21 @@
       <c r="A122" s="8" t="s">
         <v>165</v>
       </c>
+      <c r="B122" s="1">
+        <f t="shared" si="6"/>
+        <v>17062</v>
+      </c>
+      <c r="C122" s="9">
+        <f t="shared" si="7"/>
+        <v>15630</v>
+      </c>
+      <c r="D122" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E122" s="1">
+        <v>234</v>
+      </c>
       <c r="G122" s="1">
         <v>473</v>
       </c>
@@ -5067,6 +5175,21 @@
       <c r="A123" s="8" t="s">
         <v>166</v>
       </c>
+      <c r="B123" s="1">
+        <f t="shared" si="6"/>
+        <v>17192</v>
+      </c>
+      <c r="C123" s="9">
+        <f t="shared" si="7"/>
+        <v>15742</v>
+      </c>
+      <c r="D123" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E123" s="1">
+        <v>112</v>
+      </c>
       <c r="G123" s="1">
         <v>491</v>
       </c>
@@ -5075,6 +5198,21 @@
       <c r="A124" s="8" t="s">
         <v>167</v>
       </c>
+      <c r="B124" s="1">
+        <f t="shared" si="6"/>
+        <v>17384</v>
+      </c>
+      <c r="C124" s="9">
+        <f t="shared" si="7"/>
+        <v>15908</v>
+      </c>
+      <c r="D124" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E124" s="1">
+        <v>166</v>
+      </c>
       <c r="G124" s="1">
         <v>517</v>
       </c>
@@ -5083,6 +5221,21 @@
       <c r="A125" s="8" t="s">
         <v>168</v>
       </c>
+      <c r="B125" s="1">
+        <f t="shared" si="6"/>
+        <v>17701</v>
+      </c>
+      <c r="C125" s="9">
+        <f t="shared" si="7"/>
+        <v>16203</v>
+      </c>
+      <c r="D125" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E125" s="1">
+        <v>295</v>
+      </c>
       <c r="G125" s="1">
         <v>539</v>
       </c>
@@ -5091,6 +5244,21 @@
       <c r="A126" s="8" t="s">
         <v>169</v>
       </c>
+      <c r="B126" s="1">
+        <f t="shared" si="6"/>
+        <v>17913</v>
+      </c>
+      <c r="C126" s="9">
+        <f t="shared" si="7"/>
+        <v>16379</v>
+      </c>
+      <c r="D126" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E126" s="1">
+        <v>176</v>
+      </c>
       <c r="G126" s="1">
         <v>575</v>
       </c>
@@ -5099,6 +5267,21 @@
       <c r="A127" s="8" t="s">
         <v>170</v>
       </c>
+      <c r="B127" s="1">
+        <f t="shared" si="6"/>
+        <v>18045</v>
+      </c>
+      <c r="C127" s="9">
+        <f t="shared" si="7"/>
+        <v>16487</v>
+      </c>
+      <c r="D127" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E127" s="1">
+        <v>108</v>
+      </c>
       <c r="G127" s="1">
         <v>599</v>
       </c>
@@ -5107,6 +5290,21 @@
       <c r="A128" s="8" t="s">
         <v>171</v>
       </c>
+      <c r="B128" s="1">
+        <f t="shared" si="6"/>
+        <v>18186</v>
+      </c>
+      <c r="C128" s="9">
+        <f t="shared" si="7"/>
+        <v>16592</v>
+      </c>
+      <c r="D128" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E128" s="1">
+        <v>105</v>
+      </c>
       <c r="G128" s="1">
         <v>635</v>
       </c>
@@ -5115,6 +5313,21 @@
       <c r="A129" s="8" t="s">
         <v>172</v>
       </c>
+      <c r="B129" s="1">
+        <f t="shared" si="6"/>
+        <v>18345</v>
+      </c>
+      <c r="C129" s="9">
+        <f t="shared" si="7"/>
+        <v>16717</v>
+      </c>
+      <c r="D129" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E129" s="1">
+        <v>125</v>
+      </c>
       <c r="G129" s="1">
         <v>669</v>
       </c>
@@ -5123,6 +5336,21 @@
       <c r="A130" s="8" t="s">
         <v>173</v>
       </c>
+      <c r="B130" s="1">
+        <f t="shared" si="6"/>
+        <v>18764</v>
+      </c>
+      <c r="C130" s="9">
+        <f t="shared" si="7"/>
+        <v>17044</v>
+      </c>
+      <c r="D130" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E130" s="1">
+        <v>327</v>
+      </c>
       <c r="G130" s="1">
         <v>761</v>
       </c>
@@ -5131,15 +5359,66 @@
       <c r="A131" s="8" t="s">
         <v>174</v>
       </c>
+      <c r="B131" s="1">
+        <f t="shared" si="6"/>
+        <v>18983</v>
+      </c>
+      <c r="C131" s="9">
+        <f t="shared" si="7"/>
+        <v>17247</v>
+      </c>
+      <c r="D131" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E131" s="1">
+        <v>203</v>
+      </c>
+      <c r="G131" s="1">
+        <v>777</v>
+      </c>
     </row>
     <row r="132" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A132" s="8" t="s">
         <v>175</v>
       </c>
+      <c r="B132" s="1">
+        <f t="shared" si="6"/>
+        <v>19264</v>
+      </c>
+      <c r="C132" s="9">
+        <f t="shared" si="7"/>
+        <v>17482</v>
+      </c>
+      <c r="D132" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="E132" s="1">
+        <v>235</v>
+      </c>
+      <c r="G132" s="1">
+        <v>823</v>
+      </c>
     </row>
     <row r="133" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A133" s="8" t="s">
         <v>176</v>
+      </c>
+      <c r="B133" s="1">
+        <f t="shared" si="6"/>
+        <v>19275</v>
+      </c>
+      <c r="C133" s="9">
+        <f t="shared" si="7"/>
+        <v>17482</v>
+      </c>
+      <c r="D133" s="9">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="G133" s="1">
+        <v>834</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="15" x14ac:dyDescent="0.15">

</xml_diff>